<commit_message>
pixmosaic img http -> https
</commit_message>
<xml_diff>
--- a/storage/app/import/pixmosaic/pix_all.xlsx
+++ b/storage/app/import/pixmosaic/pix_all.xlsx
@@ -1615,691 +1615,691 @@
     <t>298х307</t>
   </si>
   <si>
-    <t>http://pixmosaic.ru//upload/iblock/7cf/7cf286e84c7d1071f84c85c8a460a880.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/f65/f659406ab488216b6e3bde238a8568c2.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/6ed/6edd23016c8e011dfc55b3cc79be3c1e.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/f96/f96b816695ff08528f60a1bab0900440.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/5d7/5d7a94b2fac6a08407dcd817c5af4b2d.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/f4d/f4d62a2448f916b9abf94fa6b481e29b.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/d4b/d4bb265caf0ceda033d7cf9e30cc3242.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/ffd/ffd367e899cfb8c47583cca06d631b85.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/ebc/ebc313126f282cca934de616f5a22036.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/57e/57ef82d5ad4102a933897b6e5d7209d1.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/e41/e41e7aaacf870267ad762ed40adfbc7a.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/73f/73f2efb7023eed74c6b2b54fa7824543.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/9c8/9c8ca566b67216eb30b0e8ffb5453782.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/225/2258bc716e0ed1755cb236ac3581794a.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/9a6/9a6c08e39ab51ff6867c1bb88fd98c40.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/278/2780e25a587e4f7ba57dd17b27d57282.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/1f2/1f299cde27a78a1ae0b8ea3a13f3514f.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/3c5/3c5d5bd37a5c575fcae3c4c3c214be91.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/a21/a21513720f7c687c9ce8715bb0cb8f74.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/552/5528b0f56e7cebfdbac96239a7480a4d.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/50a/50a5d7147923e4a1f9a1422a1d1030d0.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/1e7/1e70774874e705ced52bb781441054c9.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/b77/b77fb76256cb4e4e991e63ce942062e5.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/9f9/9f9bcc1d5eb79936132c6a56f2d7eba4.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/bcd/bcd94bc416e7f8c1a78c2f35720c2fc1.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/af7/af7abdfc72fc62f42c59a2d550cf4e7a.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/c2d/c2d86dd7ebf0424350033e472303f7f8.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/a77/a776fc2174e04c392e7b5e2cdf619016.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/02e/02ea163c3fad99b4d387b817b085b801.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/3c4/3c46bc55c074c0157e83da55e94d7196.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/a8e/a8e873afc554f4cbf59dbdd4b9603cb4.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/f3b/f3b4c7abeda38f6e776b616f17aa7120.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/119/1193c83c11bb88070827b0b2982090dd.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/d78/d787fcc1670c9be271d7ffde3bf516f2.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/ba8/ba827f291ca51e32729fcb0a6a973bfa.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/c83/c83c418a855580a679bba545e25045d5.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/8f3/8f352838abf29f8d6f563f813a551f19.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/91d/91d70487f42b818d8771612ca240cb30.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/1d9/1d9a96f4897484e4148e610c6812c128.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/a81/a81c68423c66853a1537f42151c80b1d.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/ec0/ec0d0badabd86feac32bdd4f17543a8d.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/420/420e66fa88b90e2633e30f30af8f2c9c.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/01c/01c93f7aba458f51e984ad3789fcd951.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/2de/2de12a719b03694d91b3947e2c815a96.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/516/5169f8b4a7176993dad3664f65cac1fd.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/040/0405f61518fe0fa2dda5e6df600a031f.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/c9c/c9cb9e1581d8cebd436227b3cd4292ff.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/89a/89a2937ca198bbc7fbca547484de5024.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/cff/cff615745bb57cddb76a91bf0681b05b.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/5d0/5d06b71a6def7f46bef0b68c8cba7f33.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/25c/25c9aa3a9a60ce470997f5995f23628c.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/1bc/1bc4caa979b92f6c712fd1c225dab658.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/4aa/4aaf20f62a445ee657c05878b9c40679.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/5ed/5ed67a1896c1c431be599bc0d1d8867e.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/3a7/3a71e95cf1bfa4fe9d70f869161c587e.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/215/215a2ef87f1cb2b3c16e3928815fc9fe.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/f24/f249381afbbfc232cf8a129950011181.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/698/698cc3b94f984f2a7331e51055a5d2a4.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/c7c/c7c996847bec41cd82810aaf4cf2eb1d.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/b65/b652d2a914b46538b8034416f56c3de7.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/a80/a80912e83a1127741709f8c69a547017.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/b24/b24d404d8d99bb184fe16a9991f79a3e.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/814/814e8169072f8caece05a7966a48da56.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/387/3879953647eb987a07c48fe8528e82d2.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/be1/be16cb91cccc277147fb0b1cba9feac3.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/89e/89ea6175826d232480d15199fd53bf36.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/688/688b33fa7231d35cc8762539e5138c39.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/65f/65fb6bdf6b1ff4a8ad6d2e70f2c855cf.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/fdb/fdb577c7b2cfe66247c7b6edc8cfcbe6.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/8e2/8e29d98c1e4ddcfdd7d840eb857e1766.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/29d/29d05edf1ab92b85e20aa4b1c442d32c.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/9bc/9bcaecd18ddeb5f2d91d9532d369a49e.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/b02/b02e97ea4326a00e10b8f0fa8ea2de4b.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/4e7/4e745bec6bce4be66129d904c8cbf255.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/420/4201ffcc60042f214efefd0ef8ecda8f.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/fc9/fc97d63a7bade88793afb6fb12b1c9a1.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/3b7/3b7b6c28d6ff3cb0d4bb87d750972a90.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/0b9/0b93b5497c0fa3f60c69c177d4fd42fd.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/58a/58a90cd16c7e6a348efd912c4af5e710.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/b91/b91eb3ef0cfb0394ae04f03c1540036b.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/cca/cca998433c5a850cf260a6170ba42586.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/f85/f850267f6a539a3893b8bb0fb246a2e4.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/8ad/8ad8ef60359ecba7b9f9f6d3e1922aae.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/410/410f3989173a29e515a8a7ca662ee71a.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/f97/f97230851e49abf4ac306a43fee729f5.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/d5f/d5fd00c44ba1b84f54e283b89cfad35a.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/181/1811a4adb84c7a5e146d733c74cf8e66.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/d0d/d0df68cc8b2dfa3eeb80117621215b6a.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/369/36986c9953fc60b26e02b74171719c75.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/1df/1df8e3bde0306d872e3a086d077e76b5.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/993/993995ec8b5ebd2b58d813e75db399fb.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/cc1/cc1c0a6d3c510f154070d6e9bc4ba7e9.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/72a/72a524165bd7e7cc7c1e9ac348cd30a6.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/6a5/6a5179f10148ba0b2190f503c97dda7d.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/7fe/7fe1633baecf5fca8c9fad14acd32737.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/a72/a728f0d4b808bf0fb7535c92c0511611.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/379/3793ffdfdebbd6aea3fc507386c4cf04.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/57c/57c2230312e95805f193f8279bc6e2f3.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/184/1845857d8cebb5282b500cd0798a4993.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/d77/d77ff7f2b335a6b86c2c25fbdf6428c4.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/de7/de77c19c69b3238af83cdbce6c143697.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/939/939a7ef3c56b9cfcd13e697f673d6d4f.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/6b0/6b0ad80e3ebde210f3dd36ece6abf663.jpeg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/ba4/ba46ee926f569444a68db9cebdbc3854.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/e83/e83c04dca533209027985ddcbe011305.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/1d8/1d82d93b9f046040f79709f0d0ff6b68.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/f57/f5747158945aaf0098813be5c5867c27.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/d6e/d6e14cafdf14fbc1dc3ab6831b6bb57e.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/221/221106b1f7e80d7dac78c6b7534f9840.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/6c9/6c9d015b331d7fd18cc5ae8a5cd91fcd.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/b50/b506c5c9df7d1251eb08af32c3e4adcd.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/cfb/cfbbbff5f9ddc09f850f4f9b35a79105.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/ace/ace04e7df37cbddb632583267162e297.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/a2d/a2db422bc83af0c936004ec49e25c919.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/1bf/1bf6c3488a1221a8632334f6d0c78ad9.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/2b4/2b4fa9af339360a870a31cba3762afaa.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/2d9/2d9f71636a6bde66b5a9785faf78efce.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/416/416ddc576a50c109d48e58716da964fb.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/1ca/1ca6bcb75f42e9d5951199a916828afa.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/26e/26e4570d95282746b0269b0f823c9821.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/0e9/0e94fabd91f94ff006f7b9e00fa4145a.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/442/442053997ac391c7299e1220b7a2a545.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/046/0460f30726112932a1b25be9ea045382.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/df9/df990eb28e6bc07d1b7f5adc9c60efd1.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/7de/7de6ce8bcb32be43e33b670366e02b6b.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/3c7/3c737681f8a9e35543217ea78bc41c1d.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/a7d/a7dd336368f60d8ecaa82d6077bcefd6.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/ddf/ddf84c7068397400ef944c88f417f338.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/bdb/bdb9a4e54203019d2fc19ce37c445b15.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/b93/b93c0579426463bcf1bfd46fe16bd3a6.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/fe1/fe1bb50c3663c12e4a713ef6377827d5.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/ce8/ce862e5e99c97baf42d58a6180331a1e.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/0d5/0d5e51e23a2153198fec4e3df56b65ec.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/b24/b24b51807ab094d86561534b861e85c5.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/07e/07e8ba9e7c997c9b44985233a885ca87.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/96b/96b24e579e6e33c3097de69f3d654200.png</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/763/763a411f05aa5131fb754e2509002c07.png</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/1da/1dae93074a302436288d897f52b41b36.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/97d/97d417e18bbada05b97a4eb3b9ba15b4.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/a23/a23039f794e7c15a21a9f1457af80844.jpeg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/378/37843f662fef4902900b51e2345c1813.jpeg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/e97/e974d516967ce3ffd13af1b2e98ec971.jpeg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/5cf/5cfe1e8f32411b82e3ed2541f0752c54.jpeg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/a4d/a4d6ecf99c61b1a06394af48875a912d.jpeg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/e1b/e1bf783603cbe2261b1efb89c0f9da24.jpeg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/ee5/ee5d6c91bc82cdaa6e13f5ca6f52feae.jpeg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/0ab/0ab3a44ffeb6bf335d7de556b0c1092f.jpeg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/4ea/4eab1f9e6384f842aa5c236b475bbb59.jpeg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/512/512a7d6c5ecaaf70e4236c33d68388c4.jpeg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/4d0/4d0113e698c245db17321ceef4a23e59.jpeg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/9e5/9e55db37747f87fce06103ce89516b0b.jpeg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/8c4/8c4c52d9bcd96a41580bcd3077cb75e1.jpeg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/8d5/8d58f48d81651755fb2afa4ed5ab102a.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/39f/39f2414efc085fa7b7f91497fe5337c1.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/04c/04c5668c87a97524295d190bbb265508.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/068/068d4710008c22f17e2dfc0b95fe6760.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/bce/bce0c5eb4d02d7292444f39c45241a00.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/a50/a50977bc20c36bc4046bda7a5620bb27.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/ea2/ea2aca7821540ce517e088c4e6eea333.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/bdb/bdbc857371b5f8e0a9c8773509ca5e2a.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/4ae/4ae37f16f3192b4ebffa42e3b9380239.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/1a5/1a54d56f38c7ec97e13be444fee6993b.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/f0e/f0e33ba5c2d4ed8ac83694b8b63084fc.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/753/7532e3d00f4ce51e4811fd38c9941613.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/530/5305cb3c65cccecd94c5c506efa05def.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/d93/d9370a3a6d9ee6d567f79274477268dd.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/2f6/2f647a708ff3b5eedc5eb2db0e2a7443.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/814/814b7f776d28fdbdea2b5b645cf7263c.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/1cf/1cf39e6f068517fe6a40e5857574de61.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/1eb/1eb5af2c7555a736483c764b8e8ef50e.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/beb/beba2cbd6f3bc19b9efb7946faacee59.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/fb6/fb6b308630a917ecce6621f93052e884.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/c83/c839abffa084692b005a456fc2dbdd75.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/5a9/5a9c8b3d9bc07690fc3ab14f560eb075.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/ecb/ecb8f869dc88fa9ae76dd3230ac82ce6.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/bc2/bc2707c86c3e5f482a2f8d94f4b37c91.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/f4f/f4f6889e1c26a6ef2f3e1396e0abe774.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/89a/89a65b69ead8c2a32fdb782fb77eac58.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/a5f/a5f2e7704baa5c4b155fba2822d8de8d.png</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/e7e/e7edf2b4a814138728a3bd82da3e4c1f.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/7f5/7f57a138e7fa6f2e92eb3557010d8580.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/86f/86fbcb40f7251a7423b3ca23bfa7d259.png</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/ee6/ee6a1000df74194656c52cef09e56b50.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/a06/a068aa0adff907e623fd36643b31eda6.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/f60/f6039e84717f2fad8476a5df8ed7a61d.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/7c1/7c18f71e8969a23345fcf4dd70aa3e62.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/3c3/3c3e7d0ccb84ed3cfaffb9370e8261e9.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/6d3/6d3d0d2ccabe70fbeb81dc8a6b9721cd.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/8bf/8bf8b3343c117a07a6f9cc2b01e323e3.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/5a4/5a4cab8fc8735462767d34ec360b3810.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/e2b/e2b844ca990c9bad5cac1df06a8c4b4b.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/053/053654e0891ef3553e9d49c2573ca51e.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/378/378b74d6da88342fa9a29e1538c0f2e8.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/f75/f7571578febb25ed5ad5c3bf55cf615c.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/aef/aef0da13cddd5665f85dd571f6170453.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/d64/d641bbca7a0335e5ed05bbc6a1a070c4.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/4ee/4ee252d60775e3106efd73235ece0552.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/4a4/4a496cfd36f0b8b60ebefc46bff78b2d.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/658/658872b983f5d947e7132694e6dcecd3.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/9e4/9e485a17f24bf029f141b981aba043f5.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/390/3903fe64cdd454f3b68c12c5c4e6f2a1.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/071/0716ffd51d8d37a7063ae89299faa6bb.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/748/7486df059a7045ae1d3b5aebe30af776.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/fe6/fe6d2c114106d2b7cbf754125bb94671.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/1d9/1d96b032845923875c0104f31d13c815.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/1f8/1f8944b44fbb4fa80c7137bef7a84dd2.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/d2b/d2b159e38c28f0f42a1454f552992177.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/469/4693ea23ee125e4f66ab53a34c073bb4.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/84e/84e39a69be2a736a01615414853fae53.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/448/4483aa893c492ce073709aac0ae99109.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/efa/efab5d344e9f664bcef53923fbb113e3.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/bb4/bb4877dfdb187af8971089fa080273a2.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/7c4/7c448b413d0c5c0e162de07de73b9f05.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/a76/a76ba3a58b72b2060d16d12498a7e303.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/c09/c09abb028986ca4367106a7cb537f9bb.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/2ef/2efe42afd823f4c0b847395b35f05d3d.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/e8b/e8b4abdf5c180ff45030f214f09eef79.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/bf9/bf984ad96a5ab71d22a37e687b8c957d.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/174/17422113cf10bf808255a31c7807d9f5.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/7d8/7d8654eac43d93fe979077700c088bef.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/9a0/9a060a3274f6e5a52af90d0879d36baf.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/e3d/e3dd5ea2813ca5e8c1d70a54fbaa754d.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/689/6897bab4b2fae4a95a7a0c96438a255b.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/8d3/8d38b7602506acd3632c5f7c25ae3885.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/c17/c17f7bf7168a4dcf40e6ffb24324df99.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/d46/d464b0758af1956d8edce07abcb24635.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/fae/fae6a494e86a88e84e0b0676794cbc7c.jpg</t>
-  </si>
-  <si>
-    <t>http://pixmosaic.ru//upload/iblock/cb9/cb9b9a799de74f0653395ce3d36a06a6.jpg</t>
-  </si>
-  <si>
     <t>img</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/7cf/7cf286e84c7d1071f84c85c8a460a880.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/f65/f659406ab488216b6e3bde238a8568c2.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/6ed/6edd23016c8e011dfc55b3cc79be3c1e.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/f96/f96b816695ff08528f60a1bab0900440.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/5d7/5d7a94b2fac6a08407dcd817c5af4b2d.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/f4d/f4d62a2448f916b9abf94fa6b481e29b.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/d4b/d4bb265caf0ceda033d7cf9e30cc3242.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/ffd/ffd367e899cfb8c47583cca06d631b85.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/ebc/ebc313126f282cca934de616f5a22036.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/57e/57ef82d5ad4102a933897b6e5d7209d1.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/e41/e41e7aaacf870267ad762ed40adfbc7a.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/73f/73f2efb7023eed74c6b2b54fa7824543.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/9c8/9c8ca566b67216eb30b0e8ffb5453782.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/225/2258bc716e0ed1755cb236ac3581794a.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/9a6/9a6c08e39ab51ff6867c1bb88fd98c40.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/278/2780e25a587e4f7ba57dd17b27d57282.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/1f2/1f299cde27a78a1ae0b8ea3a13f3514f.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/3c5/3c5d5bd37a5c575fcae3c4c3c214be91.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/a21/a21513720f7c687c9ce8715bb0cb8f74.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/552/5528b0f56e7cebfdbac96239a7480a4d.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/50a/50a5d7147923e4a1f9a1422a1d1030d0.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/1e7/1e70774874e705ced52bb781441054c9.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/b77/b77fb76256cb4e4e991e63ce942062e5.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/9f9/9f9bcc1d5eb79936132c6a56f2d7eba4.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/bcd/bcd94bc416e7f8c1a78c2f35720c2fc1.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/af7/af7abdfc72fc62f42c59a2d550cf4e7a.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/c2d/c2d86dd7ebf0424350033e472303f7f8.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/a77/a776fc2174e04c392e7b5e2cdf619016.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/02e/02ea163c3fad99b4d387b817b085b801.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/3c4/3c46bc55c074c0157e83da55e94d7196.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/a8e/a8e873afc554f4cbf59dbdd4b9603cb4.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/f3b/f3b4c7abeda38f6e776b616f17aa7120.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/119/1193c83c11bb88070827b0b2982090dd.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/d78/d787fcc1670c9be271d7ffde3bf516f2.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/ba8/ba827f291ca51e32729fcb0a6a973bfa.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/c83/c83c418a855580a679bba545e25045d5.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/8f3/8f352838abf29f8d6f563f813a551f19.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/91d/91d70487f42b818d8771612ca240cb30.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/1d9/1d9a96f4897484e4148e610c6812c128.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/a81/a81c68423c66853a1537f42151c80b1d.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/ec0/ec0d0badabd86feac32bdd4f17543a8d.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/420/420e66fa88b90e2633e30f30af8f2c9c.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/01c/01c93f7aba458f51e984ad3789fcd951.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/2de/2de12a719b03694d91b3947e2c815a96.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/516/5169f8b4a7176993dad3664f65cac1fd.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/040/0405f61518fe0fa2dda5e6df600a031f.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/c9c/c9cb9e1581d8cebd436227b3cd4292ff.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/89a/89a2937ca198bbc7fbca547484de5024.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/cff/cff615745bb57cddb76a91bf0681b05b.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/5d0/5d06b71a6def7f46bef0b68c8cba7f33.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/25c/25c9aa3a9a60ce470997f5995f23628c.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/1bc/1bc4caa979b92f6c712fd1c225dab658.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/4aa/4aaf20f62a445ee657c05878b9c40679.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/5ed/5ed67a1896c1c431be599bc0d1d8867e.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/3a7/3a71e95cf1bfa4fe9d70f869161c587e.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/215/215a2ef87f1cb2b3c16e3928815fc9fe.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/f24/f249381afbbfc232cf8a129950011181.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/698/698cc3b94f984f2a7331e51055a5d2a4.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/c7c/c7c996847bec41cd82810aaf4cf2eb1d.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/b65/b652d2a914b46538b8034416f56c3de7.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/a80/a80912e83a1127741709f8c69a547017.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/b24/b24d404d8d99bb184fe16a9991f79a3e.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/814/814e8169072f8caece05a7966a48da56.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/387/3879953647eb987a07c48fe8528e82d2.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/be1/be16cb91cccc277147fb0b1cba9feac3.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/89e/89ea6175826d232480d15199fd53bf36.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/688/688b33fa7231d35cc8762539e5138c39.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/65f/65fb6bdf6b1ff4a8ad6d2e70f2c855cf.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/fdb/fdb577c7b2cfe66247c7b6edc8cfcbe6.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/8e2/8e29d98c1e4ddcfdd7d840eb857e1766.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/29d/29d05edf1ab92b85e20aa4b1c442d32c.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/9bc/9bcaecd18ddeb5f2d91d9532d369a49e.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/b02/b02e97ea4326a00e10b8f0fa8ea2de4b.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/4e7/4e745bec6bce4be66129d904c8cbf255.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/420/4201ffcc60042f214efefd0ef8ecda8f.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/fc9/fc97d63a7bade88793afb6fb12b1c9a1.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/3b7/3b7b6c28d6ff3cb0d4bb87d750972a90.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/0b9/0b93b5497c0fa3f60c69c177d4fd42fd.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/58a/58a90cd16c7e6a348efd912c4af5e710.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/b91/b91eb3ef0cfb0394ae04f03c1540036b.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/cca/cca998433c5a850cf260a6170ba42586.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/f85/f850267f6a539a3893b8bb0fb246a2e4.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/8ad/8ad8ef60359ecba7b9f9f6d3e1922aae.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/410/410f3989173a29e515a8a7ca662ee71a.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/f97/f97230851e49abf4ac306a43fee729f5.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/d5f/d5fd00c44ba1b84f54e283b89cfad35a.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/181/1811a4adb84c7a5e146d733c74cf8e66.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/d0d/d0df68cc8b2dfa3eeb80117621215b6a.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/369/36986c9953fc60b26e02b74171719c75.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/1df/1df8e3bde0306d872e3a086d077e76b5.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/993/993995ec8b5ebd2b58d813e75db399fb.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/cc1/cc1c0a6d3c510f154070d6e9bc4ba7e9.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/72a/72a524165bd7e7cc7c1e9ac348cd30a6.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/6a5/6a5179f10148ba0b2190f503c97dda7d.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/7fe/7fe1633baecf5fca8c9fad14acd32737.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/a72/a728f0d4b808bf0fb7535c92c0511611.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/379/3793ffdfdebbd6aea3fc507386c4cf04.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/57c/57c2230312e95805f193f8279bc6e2f3.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/184/1845857d8cebb5282b500cd0798a4993.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/d77/d77ff7f2b335a6b86c2c25fbdf6428c4.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/de7/de77c19c69b3238af83cdbce6c143697.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/939/939a7ef3c56b9cfcd13e697f673d6d4f.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/6b0/6b0ad80e3ebde210f3dd36ece6abf663.jpeg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/ba4/ba46ee926f569444a68db9cebdbc3854.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/e83/e83c04dca533209027985ddcbe011305.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/1d8/1d82d93b9f046040f79709f0d0ff6b68.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/f57/f5747158945aaf0098813be5c5867c27.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/d6e/d6e14cafdf14fbc1dc3ab6831b6bb57e.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/221/221106b1f7e80d7dac78c6b7534f9840.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/6c9/6c9d015b331d7fd18cc5ae8a5cd91fcd.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/b50/b506c5c9df7d1251eb08af32c3e4adcd.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/cfb/cfbbbff5f9ddc09f850f4f9b35a79105.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/ace/ace04e7df37cbddb632583267162e297.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/a2d/a2db422bc83af0c936004ec49e25c919.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/1bf/1bf6c3488a1221a8632334f6d0c78ad9.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/2b4/2b4fa9af339360a870a31cba3762afaa.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/2d9/2d9f71636a6bde66b5a9785faf78efce.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/416/416ddc576a50c109d48e58716da964fb.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/1ca/1ca6bcb75f42e9d5951199a916828afa.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/26e/26e4570d95282746b0269b0f823c9821.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/0e9/0e94fabd91f94ff006f7b9e00fa4145a.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/442/442053997ac391c7299e1220b7a2a545.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/046/0460f30726112932a1b25be9ea045382.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/df9/df990eb28e6bc07d1b7f5adc9c60efd1.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/7de/7de6ce8bcb32be43e33b670366e02b6b.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/3c7/3c737681f8a9e35543217ea78bc41c1d.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/a7d/a7dd336368f60d8ecaa82d6077bcefd6.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/ddf/ddf84c7068397400ef944c88f417f338.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/bdb/bdb9a4e54203019d2fc19ce37c445b15.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/b93/b93c0579426463bcf1bfd46fe16bd3a6.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/fe1/fe1bb50c3663c12e4a713ef6377827d5.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/ce8/ce862e5e99c97baf42d58a6180331a1e.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/0d5/0d5e51e23a2153198fec4e3df56b65ec.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/b24/b24b51807ab094d86561534b861e85c5.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/07e/07e8ba9e7c997c9b44985233a885ca87.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/96b/96b24e579e6e33c3097de69f3d654200.png</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/763/763a411f05aa5131fb754e2509002c07.png</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/1da/1dae93074a302436288d897f52b41b36.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/97d/97d417e18bbada05b97a4eb3b9ba15b4.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/a23/a23039f794e7c15a21a9f1457af80844.jpeg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/378/37843f662fef4902900b51e2345c1813.jpeg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/e97/e974d516967ce3ffd13af1b2e98ec971.jpeg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/5cf/5cfe1e8f32411b82e3ed2541f0752c54.jpeg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/a4d/a4d6ecf99c61b1a06394af48875a912d.jpeg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/e1b/e1bf783603cbe2261b1efb89c0f9da24.jpeg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/ee5/ee5d6c91bc82cdaa6e13f5ca6f52feae.jpeg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/0ab/0ab3a44ffeb6bf335d7de556b0c1092f.jpeg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/4ea/4eab1f9e6384f842aa5c236b475bbb59.jpeg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/512/512a7d6c5ecaaf70e4236c33d68388c4.jpeg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/4d0/4d0113e698c245db17321ceef4a23e59.jpeg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/9e5/9e55db37747f87fce06103ce89516b0b.jpeg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/8c4/8c4c52d9bcd96a41580bcd3077cb75e1.jpeg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/8d5/8d58f48d81651755fb2afa4ed5ab102a.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/39f/39f2414efc085fa7b7f91497fe5337c1.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/04c/04c5668c87a97524295d190bbb265508.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/068/068d4710008c22f17e2dfc0b95fe6760.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/bce/bce0c5eb4d02d7292444f39c45241a00.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/a50/a50977bc20c36bc4046bda7a5620bb27.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/ea2/ea2aca7821540ce517e088c4e6eea333.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/bdb/bdbc857371b5f8e0a9c8773509ca5e2a.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/4ae/4ae37f16f3192b4ebffa42e3b9380239.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/1a5/1a54d56f38c7ec97e13be444fee6993b.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/f0e/f0e33ba5c2d4ed8ac83694b8b63084fc.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/753/7532e3d00f4ce51e4811fd38c9941613.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/530/5305cb3c65cccecd94c5c506efa05def.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/d93/d9370a3a6d9ee6d567f79274477268dd.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/2f6/2f647a708ff3b5eedc5eb2db0e2a7443.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/814/814b7f776d28fdbdea2b5b645cf7263c.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/1cf/1cf39e6f068517fe6a40e5857574de61.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/1eb/1eb5af2c7555a736483c764b8e8ef50e.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/beb/beba2cbd6f3bc19b9efb7946faacee59.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/fb6/fb6b308630a917ecce6621f93052e884.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/c83/c839abffa084692b005a456fc2dbdd75.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/5a9/5a9c8b3d9bc07690fc3ab14f560eb075.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/ecb/ecb8f869dc88fa9ae76dd3230ac82ce6.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/bc2/bc2707c86c3e5f482a2f8d94f4b37c91.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/f4f/f4f6889e1c26a6ef2f3e1396e0abe774.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/89a/89a65b69ead8c2a32fdb782fb77eac58.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/a5f/a5f2e7704baa5c4b155fba2822d8de8d.png</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/e7e/e7edf2b4a814138728a3bd82da3e4c1f.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/7f5/7f57a138e7fa6f2e92eb3557010d8580.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/86f/86fbcb40f7251a7423b3ca23bfa7d259.png</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/ee6/ee6a1000df74194656c52cef09e56b50.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/a06/a068aa0adff907e623fd36643b31eda6.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/f60/f6039e84717f2fad8476a5df8ed7a61d.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/7c1/7c18f71e8969a23345fcf4dd70aa3e62.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/3c3/3c3e7d0ccb84ed3cfaffb9370e8261e9.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/6d3/6d3d0d2ccabe70fbeb81dc8a6b9721cd.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/8bf/8bf8b3343c117a07a6f9cc2b01e323e3.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/5a4/5a4cab8fc8735462767d34ec360b3810.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/e2b/e2b844ca990c9bad5cac1df06a8c4b4b.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/053/053654e0891ef3553e9d49c2573ca51e.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/378/378b74d6da88342fa9a29e1538c0f2e8.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/f75/f7571578febb25ed5ad5c3bf55cf615c.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/aef/aef0da13cddd5665f85dd571f6170453.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/d64/d641bbca7a0335e5ed05bbc6a1a070c4.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/4ee/4ee252d60775e3106efd73235ece0552.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/4a4/4a496cfd36f0b8b60ebefc46bff78b2d.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/658/658872b983f5d947e7132694e6dcecd3.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/9e4/9e485a17f24bf029f141b981aba043f5.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/390/3903fe64cdd454f3b68c12c5c4e6f2a1.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/071/0716ffd51d8d37a7063ae89299faa6bb.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/748/7486df059a7045ae1d3b5aebe30af776.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/fe6/fe6d2c114106d2b7cbf754125bb94671.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/1d9/1d96b032845923875c0104f31d13c815.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/1f8/1f8944b44fbb4fa80c7137bef7a84dd2.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/d2b/d2b159e38c28f0f42a1454f552992177.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/469/4693ea23ee125e4f66ab53a34c073bb4.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/84e/84e39a69be2a736a01615414853fae53.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/448/4483aa893c492ce073709aac0ae99109.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/efa/efab5d344e9f664bcef53923fbb113e3.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/bb4/bb4877dfdb187af8971089fa080273a2.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/7c4/7c448b413d0c5c0e162de07de73b9f05.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/a76/a76ba3a58b72b2060d16d12498a7e303.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/c09/c09abb028986ca4367106a7cb537f9bb.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/2ef/2efe42afd823f4c0b847395b35f05d3d.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/e8b/e8b4abdf5c180ff45030f214f09eef79.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/bf9/bf984ad96a5ab71d22a37e687b8c957d.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/174/17422113cf10bf808255a31c7807d9f5.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/7d8/7d8654eac43d93fe979077700c088bef.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/9a0/9a060a3274f6e5a52af90d0879d36baf.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/e3d/e3dd5ea2813ca5e8c1d70a54fbaa754d.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/689/6897bab4b2fae4a95a7a0c96438a255b.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/8d3/8d38b7602506acd3632c5f7c25ae3885.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/c17/c17f7bf7168a4dcf40e6ffb24324df99.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/d46/d464b0758af1956d8edce07abcb24635.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/fae/fae6a494e86a88e84e0b0676794cbc7c.jpg</t>
+  </si>
+  <si>
+    <t>https://pixmosaic.ru//upload/iblock/cb9/cb9b9a799de74f0653395ce3d36a06a6.jpg</t>
   </si>
 </sst>
 </file>
@@ -2649,8 +2649,8 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:I233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2690,7 +2690,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>761</v>
+        <v>533</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2719,7 +2719,7 @@
         <v>465</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2748,7 +2748,7 @@
         <v>465</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2777,7 +2777,7 @@
         <v>465</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2806,7 +2806,7 @@
         <v>465</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2835,7 +2835,7 @@
         <v>465</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2864,7 +2864,7 @@
         <v>465</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2893,7 +2893,7 @@
         <v>465</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2922,7 +2922,7 @@
         <v>465</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2951,7 +2951,7 @@
         <v>465</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -2980,7 +2980,7 @@
         <v>465</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -3009,7 +3009,7 @@
         <v>465</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -3038,7 +3038,7 @@
         <v>465</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -3067,7 +3067,7 @@
         <v>465</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -3096,7 +3096,7 @@
         <v>465</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -3125,7 +3125,7 @@
         <v>465</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -3154,7 +3154,7 @@
         <v>465</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -3183,7 +3183,7 @@
         <v>465</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -3212,7 +3212,7 @@
         <v>465</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -3241,7 +3241,7 @@
         <v>465</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -3270,7 +3270,7 @@
         <v>465</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -3299,7 +3299,7 @@
         <v>465</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -3328,7 +3328,7 @@
         <v>465</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -3357,7 +3357,7 @@
         <v>465</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -3386,7 +3386,7 @@
         <v>465</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -3415,7 +3415,7 @@
         <v>469</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -3444,7 +3444,7 @@
         <v>471</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -3473,7 +3473,7 @@
         <v>473</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -3502,7 +3502,7 @@
         <v>474</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -3531,7 +3531,7 @@
         <v>471</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -3560,7 +3560,7 @@
         <v>471</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -3589,7 +3589,7 @@
         <v>471</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -3618,7 +3618,7 @@
         <v>471</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -3647,7 +3647,7 @@
         <v>476</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -3676,7 +3676,7 @@
         <v>476</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -3705,7 +3705,7 @@
         <v>476</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -3734,7 +3734,7 @@
         <v>476</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -3763,7 +3763,7 @@
         <v>476</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -3792,7 +3792,7 @@
         <v>476</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -3821,7 +3821,7 @@
         <v>469</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -3850,7 +3850,7 @@
         <v>469</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -3879,7 +3879,7 @@
         <v>469</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -3908,7 +3908,7 @@
         <v>469</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -3937,7 +3937,7 @@
         <v>480</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -3966,7 +3966,7 @@
         <v>469</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -3995,7 +3995,7 @@
         <v>483</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -4024,7 +4024,7 @@
         <v>483</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -4053,7 +4053,7 @@
         <v>484</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -4082,7 +4082,7 @@
         <v>484</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -4111,7 +4111,7 @@
         <v>486</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -4140,7 +4140,7 @@
         <v>488</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -4169,7 +4169,7 @@
         <v>488</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -4198,7 +4198,7 @@
         <v>476</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -4227,7 +4227,7 @@
         <v>491</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -4256,7 +4256,7 @@
         <v>491</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -4285,7 +4285,7 @@
         <v>476</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -4314,7 +4314,7 @@
         <v>476</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -4343,7 +4343,7 @@
         <v>495</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -4372,7 +4372,7 @@
         <v>476</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -4401,7 +4401,7 @@
         <v>476</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -4430,7 +4430,7 @@
         <v>476</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -4459,7 +4459,7 @@
         <v>476</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -4488,7 +4488,7 @@
         <v>476</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -4517,7 +4517,7 @@
         <v>476</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -4546,7 +4546,7 @@
         <v>476</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -4575,7 +4575,7 @@
         <v>476</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -4604,7 +4604,7 @@
         <v>476</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -4633,7 +4633,7 @@
         <v>476</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -4662,7 +4662,7 @@
         <v>476</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -4691,7 +4691,7 @@
         <v>476</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -4720,7 +4720,7 @@
         <v>476</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -4749,7 +4749,7 @@
         <v>476</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -4778,7 +4778,7 @@
         <v>476</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -4807,7 +4807,7 @@
         <v>500</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -4836,7 +4836,7 @@
         <v>500</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -4865,7 +4865,7 @@
         <v>500</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -4894,7 +4894,7 @@
         <v>500</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -4923,7 +4923,7 @@
         <v>500</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -4952,7 +4952,7 @@
         <v>500</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -4981,7 +4981,7 @@
         <v>476</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -5010,7 +5010,7 @@
         <v>476</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -5039,7 +5039,7 @@
         <v>476</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -5068,7 +5068,7 @@
         <v>476</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -5097,7 +5097,7 @@
         <v>476</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -5126,7 +5126,7 @@
         <v>476</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -5155,7 +5155,7 @@
         <v>476</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -5184,7 +5184,7 @@
         <v>476</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="88" spans="1:9">
@@ -5213,7 +5213,7 @@
         <v>476</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -5242,7 +5242,7 @@
         <v>476</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="90" spans="1:9">
@@ -5271,7 +5271,7 @@
         <v>476</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -5300,7 +5300,7 @@
         <v>491</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -5329,7 +5329,7 @@
         <v>506</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="93" spans="1:9">
@@ -5358,7 +5358,7 @@
         <v>506</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -5387,7 +5387,7 @@
         <v>506</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -5416,7 +5416,7 @@
         <v>506</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -5445,7 +5445,7 @@
         <v>506</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -5474,7 +5474,7 @@
         <v>506</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -5503,7 +5503,7 @@
         <v>508</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -5532,7 +5532,7 @@
         <v>506</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -5561,7 +5561,7 @@
         <v>506</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -5590,7 +5590,7 @@
         <v>506</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -5619,7 +5619,7 @@
         <v>506</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="103" spans="1:9">
@@ -5648,7 +5648,7 @@
         <v>506</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="104" spans="1:9">
@@ -5677,7 +5677,7 @@
         <v>506</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="105" spans="1:9">
@@ -5706,7 +5706,7 @@
         <v>491</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="106" spans="1:9">
@@ -5735,7 +5735,7 @@
         <v>491</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="107" spans="1:9">
@@ -5764,7 +5764,7 @@
         <v>491</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="108" spans="1:9">
@@ -5793,7 +5793,7 @@
         <v>491</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -5822,7 +5822,7 @@
         <v>491</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="110" spans="1:9">
@@ -5851,7 +5851,7 @@
         <v>491</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="111" spans="1:9">
@@ -5880,7 +5880,7 @@
         <v>491</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="112" spans="1:9">
@@ -5909,7 +5909,7 @@
         <v>491</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="113" spans="1:9">
@@ -5938,7 +5938,7 @@
         <v>491</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="114" spans="1:9">
@@ -5967,7 +5967,7 @@
         <v>491</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="115" spans="1:9">
@@ -5996,7 +5996,7 @@
         <v>491</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="116" spans="1:9">
@@ -6025,7 +6025,7 @@
         <v>491</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="117" spans="1:9">
@@ -6054,7 +6054,7 @@
         <v>491</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="118" spans="1:9">
@@ -6083,7 +6083,7 @@
         <v>491</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="119" spans="1:9">
@@ -6112,7 +6112,7 @@
         <v>491</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="120" spans="1:9">
@@ -6141,7 +6141,7 @@
         <v>476</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="121" spans="1:9">
@@ -6170,7 +6170,7 @@
         <v>476</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="122" spans="1:9">
@@ -6199,7 +6199,7 @@
         <v>476</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="123" spans="1:9">
@@ -6228,7 +6228,7 @@
         <v>476</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
     <row r="124" spans="1:9">
@@ -6257,7 +6257,7 @@
         <v>476</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="125" spans="1:9">
@@ -6286,7 +6286,7 @@
         <v>476</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="126" spans="1:9">
@@ -6315,7 +6315,7 @@
         <v>476</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
     </row>
     <row r="127" spans="1:9">
@@ -6344,7 +6344,7 @@
         <v>476</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="128" spans="1:9">
@@ -6373,7 +6373,7 @@
         <v>476</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
     </row>
     <row r="129" spans="1:9">
@@ -6402,7 +6402,7 @@
         <v>476</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="130" spans="1:9">
@@ -6431,7 +6431,7 @@
         <v>476</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="131" spans="1:9">
@@ -6460,7 +6460,7 @@
         <v>476</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row r="132" spans="1:9">
@@ -6489,7 +6489,7 @@
         <v>476</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="133" spans="1:9">
@@ -6518,7 +6518,7 @@
         <v>476</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="134" spans="1:9">
@@ -6547,7 +6547,7 @@
         <v>476</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="135" spans="1:9">
@@ -6576,7 +6576,7 @@
         <v>476</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="136" spans="1:9">
@@ -6605,7 +6605,7 @@
         <v>491</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="137" spans="1:9">
@@ -6634,7 +6634,7 @@
         <v>476</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
     </row>
     <row r="138" spans="1:9">
@@ -6663,7 +6663,7 @@
         <v>476</v>
       </c>
       <c r="I138" s="1" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
     </row>
     <row r="139" spans="1:9">
@@ -6692,7 +6692,7 @@
         <v>491</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="140" spans="1:9">
@@ -6721,7 +6721,7 @@
         <v>491</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
     </row>
     <row r="141" spans="1:9">
@@ -6750,7 +6750,7 @@
         <v>465</v>
       </c>
       <c r="I141" s="1" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
     </row>
     <row r="142" spans="1:9">
@@ -6779,7 +6779,7 @@
         <v>465</v>
       </c>
       <c r="I142" s="1" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="143" spans="1:9">
@@ -6808,7 +6808,7 @@
         <v>465</v>
       </c>
       <c r="I143" s="1" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="144" spans="1:9">
@@ -6837,7 +6837,7 @@
         <v>465</v>
       </c>
       <c r="I144" s="1" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
     </row>
     <row r="145" spans="1:9">
@@ -6866,7 +6866,7 @@
         <v>465</v>
       </c>
       <c r="I145" s="1" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="146" spans="1:9">
@@ -6895,7 +6895,7 @@
         <v>465</v>
       </c>
       <c r="I146" s="1" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
     </row>
     <row r="147" spans="1:9">
@@ -6924,7 +6924,7 @@
         <v>517</v>
       </c>
       <c r="I147" s="1" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="148" spans="1:9">
@@ -6953,7 +6953,7 @@
         <v>519</v>
       </c>
       <c r="I148" s="1" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="149" spans="1:9">
@@ -6982,7 +6982,7 @@
         <v>520</v>
       </c>
       <c r="I149" s="1" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="150" spans="1:9">
@@ -7011,7 +7011,7 @@
         <v>521</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
     </row>
     <row r="151" spans="1:9">
@@ -7040,7 +7040,7 @@
         <v>519</v>
       </c>
       <c r="I151" s="1" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="152" spans="1:9">
@@ -7069,7 +7069,7 @@
         <v>491</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="153" spans="1:9">
@@ -7098,7 +7098,7 @@
         <v>491</v>
       </c>
       <c r="I153" s="1" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="154" spans="1:9">
@@ -7127,7 +7127,7 @@
         <v>476</v>
       </c>
       <c r="I154" s="1" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
     </row>
     <row r="155" spans="1:9">
@@ -7156,7 +7156,7 @@
         <v>491</v>
       </c>
       <c r="I155" s="1" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="156" spans="1:9">
@@ -7185,7 +7185,7 @@
         <v>491</v>
       </c>
       <c r="I156" s="1" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="157" spans="1:9">
@@ -7214,7 +7214,7 @@
         <v>491</v>
       </c>
       <c r="I157" s="1" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="158" spans="1:9">
@@ -7243,7 +7243,7 @@
         <v>491</v>
       </c>
       <c r="I158" s="1" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="159" spans="1:9">
@@ -7272,7 +7272,7 @@
         <v>491</v>
       </c>
       <c r="I159" s="1" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
     </row>
     <row r="160" spans="1:9">
@@ -7301,7 +7301,7 @@
         <v>491</v>
       </c>
       <c r="I160" s="1" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="161" spans="1:9">
@@ -7330,7 +7330,7 @@
         <v>491</v>
       </c>
       <c r="I161" s="1" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
     </row>
     <row r="162" spans="1:9">
@@ -7359,7 +7359,7 @@
         <v>491</v>
       </c>
       <c r="I162" s="1" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row r="163" spans="1:9">
@@ -7388,7 +7388,7 @@
         <v>491</v>
       </c>
       <c r="I163" s="1" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="164" spans="1:9">
@@ -7417,7 +7417,7 @@
         <v>491</v>
       </c>
       <c r="I164" s="1" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
     </row>
     <row r="165" spans="1:9">
@@ -7446,7 +7446,7 @@
         <v>506</v>
       </c>
       <c r="I165" s="1" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="166" spans="1:9">
@@ -7475,7 +7475,7 @@
         <v>506</v>
       </c>
       <c r="I166" s="1" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="167" spans="1:9">
@@ -7504,7 +7504,7 @@
         <v>506</v>
       </c>
       <c r="I167" s="1" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="168" spans="1:9">
@@ -7533,7 +7533,7 @@
         <v>506</v>
       </c>
       <c r="I168" s="1" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="169" spans="1:9">
@@ -7562,7 +7562,7 @@
         <v>506</v>
       </c>
       <c r="I169" s="1" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="170" spans="1:9">
@@ -7591,7 +7591,7 @@
         <v>506</v>
       </c>
       <c r="I170" s="1" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="171" spans="1:9">
@@ -7620,7 +7620,7 @@
         <v>491</v>
       </c>
       <c r="I171" s="1" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="172" spans="1:9">
@@ -7649,7 +7649,7 @@
         <v>506</v>
       </c>
       <c r="I172" s="1" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="173" spans="1:9">
@@ -7678,7 +7678,7 @@
         <v>506</v>
       </c>
       <c r="I173" s="1" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="174" spans="1:9">
@@ -7707,7 +7707,7 @@
         <v>506</v>
       </c>
       <c r="I174" s="1" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="175" spans="1:9">
@@ -7736,7 +7736,7 @@
         <v>491</v>
       </c>
       <c r="I175" s="1" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="176" spans="1:9">
@@ -7765,7 +7765,7 @@
         <v>491</v>
       </c>
       <c r="I176" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
     </row>
     <row r="177" spans="1:9">
@@ -7794,7 +7794,7 @@
         <v>491</v>
       </c>
       <c r="I177" s="1" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="178" spans="1:9">
@@ -7823,7 +7823,7 @@
         <v>491</v>
       </c>
       <c r="I178" s="1" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
     </row>
     <row r="179" spans="1:9">
@@ -7852,7 +7852,7 @@
         <v>491</v>
       </c>
       <c r="I179" s="1" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="180" spans="1:9">
@@ -7881,7 +7881,7 @@
         <v>506</v>
       </c>
       <c r="I180" s="1" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
     </row>
     <row r="181" spans="1:9">
@@ -7910,7 +7910,7 @@
         <v>491</v>
       </c>
       <c r="I181" s="1" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="182" spans="1:9">
@@ -7939,7 +7939,7 @@
         <v>491</v>
       </c>
       <c r="I182" s="1" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
     <row r="183" spans="1:9">
@@ -7968,7 +7968,7 @@
         <v>491</v>
       </c>
       <c r="I183" s="1" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
     </row>
     <row r="184" spans="1:9">
@@ -7997,7 +7997,7 @@
         <v>491</v>
       </c>
       <c r="I184" s="1" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
     </row>
     <row r="185" spans="1:9">
@@ -8026,7 +8026,7 @@
         <v>491</v>
       </c>
       <c r="I185" s="1" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
     </row>
     <row r="186" spans="1:9">
@@ -8055,7 +8055,7 @@
         <v>491</v>
       </c>
       <c r="I186" s="1" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="187" spans="1:9">
@@ -8084,7 +8084,7 @@
         <v>491</v>
       </c>
       <c r="I187" s="1" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
     </row>
     <row r="188" spans="1:9">
@@ -8113,7 +8113,7 @@
         <v>491</v>
       </c>
       <c r="I188" s="1" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="189" spans="1:9">
@@ -8142,7 +8142,7 @@
         <v>491</v>
       </c>
       <c r="I189" s="1" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="190" spans="1:9">
@@ -8171,7 +8171,7 @@
         <v>491</v>
       </c>
       <c r="I190" s="1" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="191" spans="1:9">
@@ -8200,7 +8200,7 @@
         <v>491</v>
       </c>
       <c r="I191" s="1" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="192" spans="1:9">
@@ -8229,7 +8229,7 @@
         <v>491</v>
       </c>
       <c r="I192" s="1" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="193" spans="1:9">
@@ -8258,7 +8258,7 @@
         <v>491</v>
       </c>
       <c r="I193" s="1" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
     </row>
     <row r="194" spans="1:9">
@@ -8287,7 +8287,7 @@
         <v>506</v>
       </c>
       <c r="I194" s="1" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
     </row>
     <row r="195" spans="1:9">
@@ -8316,7 +8316,7 @@
         <v>491</v>
       </c>
       <c r="I195" s="1" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="196" spans="1:9">
@@ -8345,7 +8345,7 @@
         <v>491</v>
       </c>
       <c r="I196" s="1" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
     </row>
     <row r="197" spans="1:9">
@@ -8374,7 +8374,7 @@
         <v>506</v>
       </c>
       <c r="I197" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="198" spans="1:9">
@@ -8403,7 +8403,7 @@
         <v>506</v>
       </c>
       <c r="I198" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
     </row>
     <row r="199" spans="1:9">
@@ -8432,7 +8432,7 @@
         <v>506</v>
       </c>
       <c r="I199" s="1" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
     </row>
     <row r="200" spans="1:9">
@@ -8461,7 +8461,7 @@
         <v>506</v>
       </c>
       <c r="I200" s="1" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="201" spans="1:9">
@@ -8490,7 +8490,7 @@
         <v>506</v>
       </c>
       <c r="I201" s="1" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="202" spans="1:9">
@@ -8519,7 +8519,7 @@
         <v>506</v>
       </c>
       <c r="I202" s="1" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="203" spans="1:9">
@@ -8548,7 +8548,7 @@
         <v>491</v>
       </c>
       <c r="I203" s="1" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
     </row>
     <row r="204" spans="1:9">
@@ -8577,7 +8577,7 @@
         <v>491</v>
       </c>
       <c r="I204" s="1" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
     </row>
     <row r="205" spans="1:9">
@@ -8606,7 +8606,7 @@
         <v>491</v>
       </c>
       <c r="I205" s="1" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
     </row>
     <row r="206" spans="1:9">
@@ -8635,7 +8635,7 @@
         <v>491</v>
       </c>
       <c r="I206" s="1" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
     </row>
     <row r="207" spans="1:9">
@@ -8664,7 +8664,7 @@
         <v>491</v>
       </c>
       <c r="I207" s="1" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="208" spans="1:9">
@@ -8693,7 +8693,7 @@
         <v>491</v>
       </c>
       <c r="I208" s="1" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
     </row>
     <row r="209" spans="1:9">
@@ -8722,7 +8722,7 @@
         <v>491</v>
       </c>
       <c r="I209" s="1" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
     </row>
     <row r="210" spans="1:9">
@@ -8751,7 +8751,7 @@
         <v>491</v>
       </c>
       <c r="I210" s="1" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row r="211" spans="1:9">
@@ -8780,7 +8780,7 @@
         <v>491</v>
       </c>
       <c r="I211" s="1" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="212" spans="1:9">
@@ -8809,7 +8809,7 @@
         <v>491</v>
       </c>
       <c r="I212" s="1" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
     </row>
     <row r="213" spans="1:9">
@@ -8838,7 +8838,7 @@
         <v>491</v>
       </c>
       <c r="I213" s="1" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="214" spans="1:9">
@@ -8867,7 +8867,7 @@
         <v>491</v>
       </c>
       <c r="I214" s="1" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row r="215" spans="1:9">
@@ -8896,7 +8896,7 @@
         <v>491</v>
       </c>
       <c r="I215" s="1" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
     </row>
     <row r="216" spans="1:9">
@@ -8925,7 +8925,7 @@
         <v>491</v>
       </c>
       <c r="I216" s="1" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="217" spans="1:9">
@@ -8954,7 +8954,7 @@
         <v>491</v>
       </c>
       <c r="I217" s="1" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="218" spans="1:9">
@@ -8983,7 +8983,7 @@
         <v>506</v>
       </c>
       <c r="I218" s="1" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
     </row>
     <row r="219" spans="1:9">
@@ -9012,7 +9012,7 @@
         <v>491</v>
       </c>
       <c r="I219" s="1" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="220" spans="1:9">
@@ -9041,7 +9041,7 @@
         <v>491</v>
       </c>
       <c r="I220" s="1" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
     </row>
     <row r="221" spans="1:9">
@@ -9070,7 +9070,7 @@
         <v>491</v>
       </c>
       <c r="I221" s="1" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
     </row>
     <row r="222" spans="1:9">
@@ -9099,7 +9099,7 @@
         <v>523</v>
       </c>
       <c r="I222" s="1" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
     </row>
     <row r="223" spans="1:9">
@@ -9128,7 +9128,7 @@
         <v>523</v>
       </c>
       <c r="I223" s="1" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
     </row>
     <row r="224" spans="1:9">
@@ -9157,7 +9157,7 @@
         <v>525</v>
       </c>
       <c r="I224" s="1" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row r="225" spans="1:9">
@@ -9186,7 +9186,7 @@
         <v>526</v>
       </c>
       <c r="I225" s="1" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="226" spans="1:9">
@@ -9215,7 +9215,7 @@
         <v>528</v>
       </c>
       <c r="I226" s="3" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
     </row>
     <row r="227" spans="1:9">
@@ -9244,7 +9244,7 @@
         <v>528</v>
       </c>
       <c r="I227" s="1" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
     </row>
     <row r="228" spans="1:9">
@@ -9273,7 +9273,7 @@
         <v>530</v>
       </c>
       <c r="I228" s="1" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
     </row>
     <row r="229" spans="1:9">
@@ -9302,7 +9302,7 @@
         <v>530</v>
       </c>
       <c r="I229" s="1" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
     </row>
     <row r="230" spans="1:9">
@@ -9331,7 +9331,7 @@
         <v>530</v>
       </c>
       <c r="I230" s="1" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="231" spans="1:9">
@@ -9360,7 +9360,7 @@
         <v>532</v>
       </c>
       <c r="I231" s="1" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
     </row>
     <row r="232" spans="1:9">
@@ -9389,7 +9389,7 @@
         <v>532</v>
       </c>
       <c r="I232" s="1" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="233" spans="1:9">
@@ -9418,13 +9418,13 @@
         <v>532</v>
       </c>
       <c r="I233" s="1" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I18" r:id="rId1"/>
-    <hyperlink ref="I226" r:id="rId2"/>
+    <hyperlink ref="I18" r:id="rId1" display="http://pixmosaic.ru//upload/iblock/1f2/1f299cde27a78a1ae0b8ea3a13f3514f.jpg"/>
+    <hyperlink ref="I226" r:id="rId2" display="http://pixmosaic.ru//upload/iblock/9a0/9a060a3274f6e5a52af90d0879d36baf.jpg"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>